<commit_message>
perbaikan lap banding, kasasi, pk pada pengisian cabut
</commit_message>
<xml_diff>
--- a/hasil/2023_02_lipa_2.xlsx
+++ b/hasil/2023_02_lipa_2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>LAPORAN PERKARA YANG DIMOHONKAN BANDING</t>
   </si>
@@ -97,8 +97,8 @@
     <t>28/02/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
+    <t>01/03/2023
+01/03/2023</t>
   </si>
   <si>
     <t>688/Pdt.G/2022/PA.Tte</t>
@@ -122,6 +122,16 @@
     <t>03/02/2023</t>
   </si>
   <si>
+    <t>08/03/2023</t>
+  </si>
+  <si>
+    <t>13/03/2023</t>
+  </si>
+  <si>
+    <t>13/03/2023
+13/03/2023</t>
+  </si>
+  <si>
     <t>716/Pdt.G/2022/PA.Tte</t>
   </si>
   <si>
@@ -131,16 +141,33 @@
     <t>10/02/2023</t>
   </si>
   <si>
+    <t>07/03/2023
+03/03/2023</t>
+  </si>
+  <si>
+    <t>10/03/2023</t>
+  </si>
+  <si>
+    <t>11/04/2023</t>
+  </si>
+  <si>
+    <t>14/04/2023</t>
+  </si>
+  <si>
+    <t>17/04/2023
+17/04/2023</t>
+  </si>
+  <si>
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 10 Maret 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ketua Pengadilan Agama Ternate </t>
-  </si>
-  <si>
-    <t>Panitera</t>
+    <t>Ternate , 31 Agustus 2023</t>
+  </si>
+  <si>
+    <t>Ketua Pengadilan Agama Ternate ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panitera, </t>
   </si>
   <si>
     <t>Drs. Djabir Sasole, M.H</t>
@@ -276,10 +303,15 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -290,15 +322,10 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <left style="thin">
+      <top style="thin">
         <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="double">
+      </top>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -351,23 +378,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
@@ -375,7 +402,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
@@ -684,20 +711,20 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="13.2" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="13.15" defaultColWidth="8.85546875" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="true" style="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="true" style="1"/>
-    <col min="3" max="3" width="29.88671875" customWidth="true" style="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="true" style="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="true" style="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="true" style="1"/>
-    <col min="7" max="7" width="11.77734375" customWidth="true" style="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="true" style="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="true" style="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="true" style="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="true" style="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="true" style="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="true" style="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true" style="1"/>
     <col min="8" max="8" width="12" customWidth="true" style="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="true" style="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="true" style="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="true" style="1"/>
-    <col min="12" max="12" width="8.5546875" customWidth="true" style="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="true" style="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="true" style="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="true" style="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="true" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" customHeight="1" ht="15.6">
@@ -771,68 +798,68 @@
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:16" customHeight="1" ht="31.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
+    <row r="6" spans="1:16" customHeight="1" ht="31.15">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="13"/>
-    </row>
-    <row r="7" spans="1:16" customHeight="1" ht="28.8">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:16" customHeight="1" ht="16.2">
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" customHeight="1" ht="28.9">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:16" customHeight="1" ht="16.15">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -926,10 +953,14 @@
       <c r="G10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="H10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="J10" s="17" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -939,25 +970,31 @@
         <v>3</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+        <v>38</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="J11" s="17" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
@@ -994,7 +1031,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1002,7 +1039,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -1012,7 +1049,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1020,7 +1057,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1087,7 +1124,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1095,7 +1132,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -1105,7 +1142,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1113,13 +1150,13 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:16" customHeight="1" ht="19.95">
+    <row r="22" spans="1:16" customHeight="1" ht="19.9">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
@@ -1133,7 +1170,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:16" customHeight="1" ht="19.95">
+    <row r="23" spans="1:16" customHeight="1" ht="19.9">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -1203,7 +1240,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
     </row>
-    <row r="28" spans="1:16" customHeight="1" ht="19.95">
+    <row r="28" spans="1:16" customHeight="1" ht="19.9">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
@@ -1217,7 +1254,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:16" customHeight="1" ht="19.95">
+    <row r="29" spans="1:16" customHeight="1" ht="19.9">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -2372,8 +2409,8 @@
     <mergeCell ref="L5:L7"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="1.46" right="0.19685039370079" top="0.43307086614173" bottom="0.43307086614173" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="5" orientation="landscape" scale="95" fitToHeight="1" fitToWidth="1"/>
+  <pageMargins left="0.98425196850394" right="0.39370078740157" top="0.31496062992126" bottom="0.23622047244094" header="0" footer="0"/>
+  <pageSetup paperSize="14" orientation="landscape" scale="79" fitToHeight="1" fitToWidth="1"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>